<commit_message>
update final ajout front
frrront
</commit_message>
<xml_diff>
--- a/gestionEve_Spon/Détails sponsor.xlsx
+++ b/gestionEve_Spon/Détails sponsor.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Nom</t>
   </si>
@@ -38,13 +38,16 @@
     <t>ooo</t>
   </si>
   <si>
-    <t>oooooooooYYY</t>
+    <t>sdfsd</t>
   </si>
   <si>
-    <t>VVV</t>
+    <t>sdf</t>
   </si>
   <si>
-    <t>VV</t>
+    <t>sfdfds</t>
+  </si>
+  <si>
+    <t>dsds</t>
   </si>
 </sst>
 </file>
@@ -137,13 +140,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>55.0</v>
+        <v>4774.0</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>